<commit_message>
Se adiciono gitignore, AppData
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Refineries_FlexStart.xlsx
+++ b/SuppXLS/Scen_Refineries_FlexStart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Music\TIMES-O-G-B\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Pictures\ModeloTIMESOG\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562DC1AB-CC92-435F-83E6-D2353F06D1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50378C24-ADE3-4D33-AFC4-BB19F281B310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="45" windowWidth="20295" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="45" windowWidth="20190" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuels" sheetId="7" r:id="rId1"/>
@@ -696,8 +696,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
@@ -1259,7 +1258,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>

</xml_diff>

<commit_message>
Cambio nombres en BASE, hojas "COMM" y "PROCESS"
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Refineries_FlexStart.xlsx
+++ b/SuppXLS/Scen_Refineries_FlexStart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Pictures\ModeloTIMESOG\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scaic\OneDrive\Documentos\GitHub\ModeloTIMESOG\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50378C24-ADE3-4D33-AFC4-BB19F281B310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07177A55-9AE5-4EEC-8108-146B6AD0CF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="45" windowWidth="20190" windowHeight="10875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuels" sheetId="7" r:id="rId1"/>
@@ -3821,7 +3821,7 @@
         <v>2019</v>
       </c>
       <c r="H9" s="24">
-        <v>2.6523215703436E-2</v>
+        <v>9.0891443724778007E-3</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>25</v>
@@ -3847,7 +3847,7 @@
         <v>2019</v>
       </c>
       <c r="H10" s="24">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>25</v>
@@ -4092,7 +4092,7 @@
         <v>2019</v>
       </c>
       <c r="H20" s="24">
-        <v>0.31052010338168201</v>
+        <v>0.31202149152079001</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>37</v>
@@ -4118,7 +4118,7 @@
         <v>2019</v>
       </c>
       <c r="H21" s="24">
-        <v>0.335419513504495</v>
+        <v>0.337041292171051</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>37</v>
@@ -4144,7 +4144,7 @@
         <v>2019</v>
       </c>
       <c r="H22" s="24">
-        <v>8.3862120957725605E-2</v>
+        <v>8.4267600642793303E-2</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>37</v>
@@ -4170,7 +4170,7 @@
         <v>2019</v>
       </c>
       <c r="H23" s="24">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>37</v>
@@ -4196,7 +4196,7 @@
         <v>2019</v>
       </c>
       <c r="H24" s="24">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>37</v>
@@ -4222,7 +4222,7 @@
         <v>2019</v>
       </c>
       <c r="H25" s="24">
-        <v>3.2377019198036198E-2</v>
+        <v>2.6675609175347101E-2</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>37</v>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="J7" s="119">
         <f>I7/SUM($I$7:$I$11)</f>
-        <v>0.2488261971401039</v>
+        <v>0.25039392243497394</v>
       </c>
       <c r="K7" s="129"/>
       <c r="L7" s="99"/>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="J8" s="119">
         <f t="shared" ref="J8:J11" si="0">I8/SUM($I$7:$I$11)</f>
-        <v>0.63557675031598704</v>
+        <v>0.63958119100492561</v>
       </c>
       <c r="K8" s="130"/>
       <c r="L8" s="99"/>
@@ -4774,7 +4774,7 @@
       </c>
       <c r="J9" s="119">
         <f t="shared" si="0"/>
-        <v>6.8982780040473396E-2</v>
+        <v>6.9417404892771456E-2</v>
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="99"/>
@@ -4846,15 +4846,15 @@
       </c>
       <c r="H10" s="123">
         <f>Refineries_Base!H9</f>
-        <v>2.6523215703436E-2</v>
+        <v>9.0891443724778007E-3</v>
       </c>
       <c r="I10" s="120">
         <f>H10*$G$3*1000/Fuels!$F$32</f>
-        <v>653.28117496147786</v>
+        <v>223.87055104625128</v>
       </c>
       <c r="J10" s="119">
         <f t="shared" si="0"/>
-        <v>3.7148231892137035E-2</v>
+        <v>1.2810398911526513E-2</v>
       </c>
       <c r="K10" s="130"/>
       <c r="L10" s="99"/>
@@ -4899,15 +4899,15 @@
       </c>
       <c r="H11" s="123">
         <f>Refineries_Base!H10</f>
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="I11" s="120">
         <f>H11*$G$3*1000/Fuels!$F$33</f>
-        <v>166.46784564977659</v>
+        <v>485.77318138161172</v>
       </c>
       <c r="J11" s="119">
         <f t="shared" si="0"/>
-        <v>9.4660406112988451E-3</v>
+        <v>2.7797082755802567E-2</v>
       </c>
       <c r="K11" s="130"/>
       <c r="L11" s="99"/>
@@ -5293,7 +5293,7 @@
       </c>
       <c r="M24" s="119">
         <f>L24/SUM($L$24:$L$28)</f>
-        <v>0.32836672697869629</v>
+        <v>0.31935312232852886</v>
       </c>
       <c r="N24" s="99"/>
       <c r="P24" t="str">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="M25" s="119">
         <f>L25/SUM($L$24:$L$28)</f>
-        <v>0.5300502223565402</v>
+        <v>0.51550044384208926</v>
       </c>
       <c r="N25" s="99"/>
       <c r="P25" t="str">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="M26" s="119">
         <f>L26/SUM($L$24:$L$28)</f>
-        <v>0.10509650718287038</v>
+        <v>0.10221162790604484</v>
       </c>
       <c r="N26" s="99"/>
       <c r="P26" t="str">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="M27" s="119">
         <f>L27/SUM($L$24:$L$28)</f>
-        <v>2.1771839762109411E-2</v>
+        <v>2.1174206871809959E-2</v>
       </c>
       <c r="N27" s="99"/>
       <c r="P27" t="str">
@@ -5465,15 +5465,15 @@
       </c>
       <c r="K28" s="173">
         <f>H11</f>
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="L28" s="120">
         <f>K28*$G$3*1000/Fuels!$F$33</f>
-        <v>166.46784564977659</v>
+        <v>485.77318138161172</v>
       </c>
       <c r="M28" s="119">
         <f>L28/SUM($L$24:$L$28)</f>
-        <v>1.471470371978382E-2</v>
+        <v>4.1760599051527118E-2</v>
       </c>
       <c r="N28" s="99"/>
       <c r="P28" t="str">
@@ -5536,7 +5536,7 @@
       <c r="J31" s="100"/>
       <c r="K31" s="156">
         <f>SUM(K24:K30)</f>
-        <v>0.61308914437247786</v>
+        <v>0.63052321570343606</v>
       </c>
       <c r="M31" s="27"/>
       <c r="N31" s="99"/>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="K42" s="152"/>
       <c r="L42" s="154">
-        <v>2.6523215703436E-2</v>
+        <v>9.0891443724778007E-3</v>
       </c>
       <c r="M42" s="152"/>
       <c r="N42" s="152" t="s">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="K43" s="152"/>
       <c r="L43" s="154">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="M43" s="152"/>
       <c r="N43" s="152" t="s">
@@ -8689,7 +8689,7 @@
         <v>26</v>
       </c>
       <c r="L112" s="7">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="N112" t="s">
         <v>25</v>
@@ -8884,7 +8884,7 @@
       </c>
       <c r="K119" s="152"/>
       <c r="L119" s="154">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="M119" s="152"/>
       <c r="N119" s="152" t="s">
@@ -9077,7 +9077,7 @@
         <v>26</v>
       </c>
       <c r="L126" s="7">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="N126" t="s">
         <v>25</v>
@@ -9272,7 +9272,7 @@
       </c>
       <c r="K133" s="152"/>
       <c r="L133" s="154">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="M133" s="152"/>
       <c r="N133" s="152" t="s">
@@ -9465,7 +9465,7 @@
         <v>26</v>
       </c>
       <c r="L140" s="7">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="N140" t="s">
         <v>25</v>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="K147" s="152"/>
       <c r="L147" s="154">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="M147" s="152"/>
       <c r="N147" s="152" t="s">
@@ -9853,7 +9853,7 @@
         <v>26</v>
       </c>
       <c r="L154" s="7">
-        <v>9.0891443724778007E-3</v>
+        <v>2.6523215703436E-2</v>
       </c>
       <c r="N154" t="s">
         <v>25</v>
@@ -10107,15 +10107,15 @@
       </c>
       <c r="I7" s="123">
         <f>Refineries_Base!H20</f>
-        <v>0.31052010338168201</v>
+        <v>0.31202149152079001</v>
       </c>
       <c r="J7" s="118">
         <f>I7*$H$3*1000/Fuels!$F$29</f>
-        <v>5825.8931216075425</v>
+        <v>5854.0617546114445</v>
       </c>
       <c r="K7" s="119">
         <f>J7/SUM($J$7:$J$11)</f>
-        <v>0.32400441593000112</v>
+        <v>0.30154280207718515</v>
       </c>
       <c r="L7" s="127">
         <v>0</v>
@@ -10190,15 +10190,15 @@
       </c>
       <c r="I8" s="123">
         <f>Refineries_Base!H21</f>
-        <v>0.335419513504495</v>
+        <v>0.337041292171051</v>
       </c>
       <c r="J8" s="120">
         <f>I8*$H$3*1000/Fuels!$F$30</f>
-        <v>5915.6880688623469</v>
+        <v>5944.290867214303</v>
       </c>
       <c r="K8" s="119">
         <f t="shared" ref="K8:K11" si="1">J8/SUM($J$7:$J$11)</f>
-        <v>0.32899832138474627</v>
+        <v>0.30619050491731514</v>
       </c>
       <c r="L8" s="127">
         <v>0</v>
@@ -10273,15 +10273,15 @@
       </c>
       <c r="I9" s="123">
         <f>Refineries_Base!H22</f>
-        <v>8.3862120957725605E-2</v>
+        <v>8.4267600642793303E-2</v>
       </c>
       <c r="J9" s="120">
         <f>I9*$H$3*1000/Fuels!$F$31</f>
-        <v>1780.5121222447049</v>
+        <v>1789.1210327556962</v>
       </c>
       <c r="K9" s="119">
         <f t="shared" si="1"/>
-        <v>9.9022377888216329E-2</v>
+        <v>9.2157649182193907E-2</v>
       </c>
       <c r="L9" s="127">
         <v>0</v>
@@ -10356,15 +10356,15 @@
       </c>
       <c r="I10" s="123">
         <f>Refineries_Base!H23</f>
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="J10" s="120">
         <f>I10*$H$3*1000/Fuels!$F$32</f>
-        <v>402.13994923467499</v>
+        <v>5579.8570480084491</v>
       </c>
       <c r="K10" s="119">
         <f t="shared" si="1"/>
-        <v>2.236483173552431E-2</v>
+        <v>0.2874185138414681</v>
       </c>
       <c r="L10" s="127">
         <v>0</v>
@@ -10412,15 +10412,15 @@
       </c>
       <c r="I11" s="123">
         <f>Refineries_Base!H24</f>
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="J11" s="120">
         <f>I11*$H$3*1000/Fuels!$F$33</f>
-        <v>4056.6732787386995</v>
+        <v>246.37015276328938</v>
       </c>
       <c r="K11" s="119">
         <f t="shared" si="1"/>
-        <v>0.22561005306151191</v>
+        <v>1.2690529981837784E-2</v>
       </c>
       <c r="L11" s="127">
         <v>0</v>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="I12" s="124">
         <f>Refineries_Base!H25</f>
-        <v>3.2377019198036198E-2</v>
+        <v>2.6675609175347101E-2</v>
       </c>
       <c r="J12" s="157"/>
       <c r="K12" s="158"/>
@@ -10601,7 +10601,7 @@
       <c r="F14" s="95"/>
       <c r="I14" s="6">
         <f>SUM(I7:I13)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
       <c r="K14" s="17"/>
       <c r="M14" s="99"/>
@@ -10807,7 +10807,7 @@
       </c>
       <c r="K24" s="119">
         <f>J24/SUM($J$24:$J$28)</f>
-        <v>0.33066370734221712</v>
+        <v>0.30759916555131789</v>
       </c>
       <c r="L24" s="168">
         <f>R7</f>
@@ -10819,7 +10819,7 @@
       </c>
       <c r="N24" s="119">
         <f>M24/SUM($M$24:$M$28)</f>
-        <v>0.34167890403729334</v>
+        <v>0.25964727638840557</v>
       </c>
       <c r="O24" s="99"/>
       <c r="Q24" t="str">
@@ -10851,7 +10851,7 @@
       </c>
       <c r="K25" s="119">
         <f>J25/SUM($J$24:$J$28)</f>
-        <v>0.33113902209217527</v>
+        <v>0.30804132602195594</v>
       </c>
       <c r="L25" s="169">
         <f>R8</f>
@@ -10863,7 +10863,7 @@
       </c>
       <c r="N25" s="119">
         <f>M25/SUM($M$24:$M$28)</f>
-        <v>0.35411685023050926</v>
+        <v>0.26909907108446196</v>
       </c>
       <c r="O25" s="99"/>
       <c r="Q25" t="str">
@@ -10895,7 +10895,7 @@
       </c>
       <c r="K26" s="119">
         <f>J26/SUM($J$24:$J$28)</f>
-        <v>9.3697224278935745E-2</v>
+        <v>8.7161630873651086E-2</v>
       </c>
       <c r="L26" s="169">
         <f>R9</f>
@@ -10907,7 +10907,7 @@
       </c>
       <c r="N26" s="119">
         <f>M26/SUM($M$24:$M$28)</f>
-        <v>0.10312717369672739</v>
+        <v>7.8367992450206064E-2</v>
       </c>
       <c r="O26" s="99"/>
       <c r="Q26" t="str">
@@ -10918,11 +10918,11 @@
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f>I27</f>
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="B27" s="6">
         <f>B26+A27</f>
-        <v>0.76061295224244296</v>
+        <v>0.97082826645265818</v>
       </c>
       <c r="E27" s="174">
         <f>R10</f>
@@ -10935,27 +10935,27 @@
       </c>
       <c r="I27" s="180">
         <f>I10</f>
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="J27" s="120">
         <f>I27*$H$3*1000/Fuels!$F$32</f>
-        <v>402.13994923467499</v>
+        <v>5579.8570480084491</v>
       </c>
       <c r="K27" s="119">
         <f>J27/SUM($J$24:$J$28)</f>
-        <v>2.2051436374312519E-2</v>
+        <v>0.28463045030204409</v>
       </c>
       <c r="L27" s="173">
         <f>I10</f>
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="M27" s="120">
         <f>L27*$H$3*1000/Fuels!$F$32</f>
-        <v>402.13994923467499</v>
+        <v>5579.8570480084491</v>
       </c>
       <c r="N27" s="119">
         <f>M27/SUM($M$24:$M$28)</f>
-        <v>2.4537847244908567E-2</v>
+        <v>0.25873067318435927</v>
       </c>
       <c r="O27" s="99"/>
       <c r="Q27" t="b">
@@ -10966,11 +10966,11 @@
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <f>I12</f>
-        <v>3.2377019198036198E-2</v>
+        <v>2.6675609175347101E-2</v>
       </c>
       <c r="B28" s="6">
         <f>B27+A28</f>
-        <v>0.79298997144047911</v>
+        <v>0.99750387562800524</v>
       </c>
       <c r="D28" s="174">
         <f>S11</f>
@@ -10983,15 +10983,15 @@
       </c>
       <c r="I28" s="172">
         <f>I11</f>
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="J28" s="120">
         <f>I28*$H$3*1000/Fuels!$F$33</f>
-        <v>4056.6732787386995</v>
+        <v>246.37015276328938</v>
       </c>
       <c r="K28" s="119">
         <f>J28/SUM($J$24:$J$28)</f>
-        <v>0.22244860991235929</v>
+        <v>1.2567427251030942E-2</v>
       </c>
       <c r="L28" s="169">
         <f>R11</f>
@@ -11003,12 +11003,12 @@
       </c>
       <c r="N28" s="119">
         <f>M28/SUM($M$24:$M$28)</f>
-        <v>0.17653922479056142</v>
+        <v>0.13415498689256705</v>
       </c>
       <c r="O28" s="99"/>
-      <c r="Q28" t="str">
+      <c r="Q28" t="b">
         <f t="shared" si="4"/>
-        <v>Sí</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
@@ -11058,18 +11058,18 @@
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <f>100%-B28</f>
-        <v>0.20701002855952089</v>
+        <v>2.4961243719947568E-3</v>
       </c>
       <c r="F31" s="95"/>
       <c r="I31" s="128">
         <f>SUM(I24:I30)</f>
-        <v>1.4831073132615757</v>
+        <v>1.4852800767935337</v>
       </c>
       <c r="J31" s="100"/>
       <c r="K31" s="100"/>
       <c r="L31" s="156">
         <f>SUM(L24:L30)</f>
-        <v>0.88141731496057885</v>
+        <v>1.0916326291707941</v>
       </c>
       <c r="N31" s="27"/>
       <c r="O31" s="99"/>
@@ -11295,7 +11295,7 @@
       <c r="L39" s="145"/>
       <c r="M39" s="147" cm="1">
         <f t="array" ref="M39:M45">+IF(J39&lt;$H$34,$I$7:$I$13,$I$24:$I$30)</f>
-        <v>0.31052010338168201</v>
+        <v>0.31202149152079001</v>
       </c>
       <c r="N39" s="145"/>
       <c r="O39" s="145" t="s">
@@ -11373,7 +11373,7 @@
       </c>
       <c r="L40" s="152"/>
       <c r="M40" s="154">
-        <v>0.335419513504495</v>
+        <v>0.337041292171051</v>
       </c>
       <c r="N40" s="152"/>
       <c r="O40" s="152" t="s">
@@ -11446,7 +11446,7 @@
       </c>
       <c r="L41" s="152"/>
       <c r="M41" s="154">
-        <v>8.3862120957725605E-2</v>
+        <v>8.4267600642793303E-2</v>
       </c>
       <c r="N41" s="152"/>
       <c r="O41" s="152" t="s">
@@ -11519,7 +11519,7 @@
       </c>
       <c r="L42" s="152"/>
       <c r="M42" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N42" s="152"/>
       <c r="O42" s="152" t="s">
@@ -11592,7 +11592,7 @@
       </c>
       <c r="L43" s="152"/>
       <c r="M43" s="154">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="N43" s="152"/>
       <c r="O43" s="152" t="s">
@@ -11665,7 +11665,7 @@
       </c>
       <c r="L44" s="152"/>
       <c r="M44" s="154">
-        <v>3.2377019198036198E-2</v>
+        <v>2.6675609175347101E-2</v>
       </c>
       <c r="N44" s="152"/>
       <c r="O44" s="152" t="s">
@@ -11895,7 +11895,7 @@
         <v>26</v>
       </c>
       <c r="M49" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O49" t="s">
         <v>37</v>
@@ -11919,7 +11919,7 @@
         <v>26</v>
       </c>
       <c r="M50" s="7">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="O50" t="s">
         <v>37</v>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="L56" s="152"/>
       <c r="M56" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N56" s="152"/>
       <c r="O56" s="152" t="s">
@@ -12301,7 +12301,7 @@
       </c>
       <c r="L57" s="152"/>
       <c r="M57" s="154">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="N57" s="152"/>
       <c r="O57" s="152" t="s">
@@ -12613,7 +12613,7 @@
         <v>26</v>
       </c>
       <c r="M63" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O63" t="s">
         <v>37</v>
@@ -12637,7 +12637,7 @@
         <v>26</v>
       </c>
       <c r="M64" s="7">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="O64" t="s">
         <v>37</v>
@@ -13036,7 +13036,7 @@
       </c>
       <c r="L70" s="152"/>
       <c r="M70" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N70" s="152"/>
       <c r="O70" s="152" t="s">
@@ -13112,7 +13112,7 @@
       </c>
       <c r="L71" s="152"/>
       <c r="M71" s="154">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="N71" s="152"/>
       <c r="O71" s="152" t="s">
@@ -13365,7 +13365,7 @@
         <v>26</v>
       </c>
       <c r="M77" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O77" t="s">
         <v>37</v>
@@ -13389,7 +13389,7 @@
         <v>26</v>
       </c>
       <c r="M78" s="7">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="O78" t="s">
         <v>37</v>
@@ -13558,7 +13558,7 @@
       </c>
       <c r="L84" s="152"/>
       <c r="M84" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N84" s="152"/>
       <c r="O84" s="152" t="s">
@@ -13588,7 +13588,7 @@
       </c>
       <c r="L85" s="152"/>
       <c r="M85" s="154">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="N85" s="152"/>
       <c r="O85" s="152" t="s">
@@ -13755,7 +13755,7 @@
         <v>26</v>
       </c>
       <c r="M91" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O91" t="s">
         <v>37</v>
@@ -13779,7 +13779,7 @@
         <v>26</v>
       </c>
       <c r="M92" s="7">
-        <v>0.221494361019133</v>
+        <v>1.34518103408756E-2</v>
       </c>
       <c r="O92" t="s">
         <v>37</v>
@@ -14201,7 +14201,7 @@
         <v>26</v>
       </c>
       <c r="M111" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O111" t="s">
         <v>37</v>
@@ -14390,7 +14390,7 @@
       </c>
       <c r="L118" s="152"/>
       <c r="M118" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N118" s="152"/>
       <c r="O118" s="152" t="s">
@@ -14589,7 +14589,7 @@
         <v>26</v>
       </c>
       <c r="M125" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O125" t="s">
         <v>37</v>
@@ -14778,7 +14778,7 @@
       </c>
       <c r="L132" s="152"/>
       <c r="M132" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N132" s="152"/>
       <c r="O132" s="152" t="s">
@@ -14977,7 +14977,7 @@
         <v>26</v>
       </c>
       <c r="M139" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O139" t="s">
         <v>37</v>
@@ -15166,7 +15166,7 @@
       </c>
       <c r="L146" s="152"/>
       <c r="M146" s="154">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="N146" s="152"/>
       <c r="O146" s="152" t="s">
@@ -15365,7 +15365,7 @@
         <v>26</v>
       </c>
       <c r="M153" s="7">
-        <v>1.6326881938927802E-2</v>
+        <v>0.226542196149143</v>
       </c>
       <c r="O153" t="s">
         <v>37</v>

</xml_diff>